<commit_message>
Changes for new model
</commit_message>
<xml_diff>
--- a/Modelo_Excel.xlsx
+++ b/Modelo_Excel.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC19F6D1-939D-432C-8C0A-8CA1A8E004D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78CB620-21E1-4175-9D9A-535327A19DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{887467BD-7735-420A-AF4C-622F021D4341}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{21E64127-3ADB-49F3-A7B0-7732C79B9E91}"/>
   </bookViews>
   <sheets>
-    <sheet name="Grado x" sheetId="1" r:id="rId1"/>
-    <sheet name="Grado xx" sheetId="2" r:id="rId2"/>
+    <sheet name="Primer Grado" sheetId="1" r:id="rId1"/>
+    <sheet name="Segundo Grado" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,39 +37,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Alumno</t>
   </si>
   <si>
-    <t>Curso A</t>
+    <t>Matematica</t>
   </si>
   <si>
-    <t>Curso B</t>
+    <t>Comunicación</t>
   </si>
   <si>
-    <t>Curso C</t>
-  </si>
-  <si>
-    <t>Curso D</t>
-  </si>
-  <si>
-    <t>Curso E</t>
-  </si>
-  <si>
-    <t>Curso F</t>
+    <t>Ingles</t>
   </si>
   <si>
     <t>Mark</t>
   </si>
   <si>
     <t>Jose</t>
-  </si>
-  <si>
-    <t>a'</t>
-  </si>
-  <si>
-    <t>f</t>
   </si>
 </sst>
 </file>
@@ -110,7 +95,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,74 +411,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B644A4-2AA6-48E1-8C65-04DA383060F0}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080F5B4E-4E76-44E7-A36C-C823BB98873A}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2">
         <v>14</v>
       </c>
       <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>23</v>
-      </c>
-      <c r="F2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
         <v>12</v>
       </c>
-      <c r="G2">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3">
-        <v>-23</v>
-      </c>
-      <c r="E3">
-        <v>23</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -500,14 +469,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B2BF9D-EC0F-44A5-A482-F460B06ADAE0}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD7BE11-83CD-484B-8339-B4C5E439CC62}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,60 +492,33 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
       <c r="B2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2">
-        <v>34</v>
-      </c>
-      <c r="E2">
         <v>12</v>
       </c>
-      <c r="F2">
-        <v>34</v>
-      </c>
-      <c r="G2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>-14</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>